<commit_message>
Assignment 2 - ThreeSum Problem (BenchmarkingUpdate)
</commit_message>
<xml_diff>
--- a/Assignment2 Reports/ThreeSum_Benchmarking.xlsx
+++ b/Assignment2 Reports/ThreeSum_Benchmarking.xlsx
@@ -8,14 +8,63 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vipulrajderkar/MSIS/PSA/PSA-INFO6205/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE8B8ECF-C7F3-8247-A8F4-61126AD4EF08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEB4BF2-ADD8-E246-A548-BA879EB218EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10160" yWindow="0" windowWidth="28240" windowHeight="21600" xr2:uid="{9BE36209-CEBA-8A46-A923-76A25FA9FF80}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{9BE36209-CEBA-8A46-A923-76A25FA9FF80}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$H$3</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$H$4:$H$10</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$I$3</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$I$4:$I$10</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$J$3</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$J$4:$J$10</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$K$3</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$K$4:$K$10</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$L$3</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$L$4:$L$10</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$B$4:$B$10</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$C$3</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$C$4:$C$10</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$D$3</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$D$4:$D$10</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$E$3</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$E$4:$E$10</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$F$3</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$F$4:$F$10</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$B$4:$B$10</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$C$3</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$C$4:$C$10</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$D$3</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$D$4:$D$10</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$E$3</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$E$4:$E$10</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$F$3</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$F$4:$F$10</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$B$4:$B$10</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$C$3</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$C$4:$C$10</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$D$3</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$D$4:$D$10</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$E$3</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$E$4:$E$10</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$F$3</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$F$4:$F$10</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$H$3</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$H$4:$H$10</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">Sheet1!$I$3</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">Sheet1!$I$4:$I$10</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">Sheet1!$J$3</definedName>
+    <definedName name="_xlchart.v2.5" hidden="1">Sheet1!$J$4:$J$10</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">Sheet1!$K$3</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">Sheet1!$K$4:$K$10</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">Sheet1!$L$3</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">Sheet1!$L$4:$L$10</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>N</t>
   </si>
@@ -52,12 +101,15 @@
   <si>
     <t>Quadratic with Calipers(ms)</t>
   </si>
+  <si>
+    <t>Log Scale</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +117,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,8 +150,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,7 +255,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Sheet1!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -256,7 +326,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Sheet1!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -286,7 +356,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:f>Sheet1!$C$4:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -579,7 +649,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Sheet1!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -650,7 +720,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Sheet1!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -680,7 +750,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$9</c:f>
+              <c:f>Sheet1!$D$4:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -973,7 +1043,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Sheet1!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1044,7 +1114,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Sheet1!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1074,7 +1144,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$9</c:f>
+              <c:f>Sheet1!$E$4:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1367,7 +1437,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
+              <c:f>Sheet1!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1438,7 +1508,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>Sheet1!$B$4:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1468,7 +1538,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$9</c:f>
+              <c:f>Sheet1!$F$4:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1489,6 +1559,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>161619</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1285873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1678,6 +1751,847 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Complexity Comparison (Log scale)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quadratic(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.965784284662087</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$4:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.87970576628228825</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6507645591169022</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7655347463629774</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8176232575114311</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.2211037253678763</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.4234731247064101</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.386131937314994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-58AD-0542-A63C-A522F2E955D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quadratic with Calipers(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.965784284662087</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.12432813500220179</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.18903382439001684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0874628412503395</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2479275134435852</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5204222485264456</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.0434921530640615</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.144339591247839</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-58AD-0542-A63C-A522F2E955D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quadrithimic(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent3">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.965784284662087</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$4:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.11103131238874395</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5260688116675876</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8328900141647417</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1578521691417381</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3776443583999072</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10.517994105587512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.749869427396845</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-58AD-0542-A63C-A522F2E955D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cubic(ms)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$4:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>7.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.965784284662087</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.965784284662087</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$4:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>2.5777309314900805</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3462477740827756</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3124292062506147</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.298463578910917</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.288260499528787</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.30223728635373</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.294316730405338</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-58AD-0542-A63C-A522F2E955D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1734265264"/>
+        <c:axId val="40700655"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1734265264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="40700655"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="40700655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1734265264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
   <a:schemeClr val="accent1"/>
@@ -1826,6 +2740,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
   <cs:axisTitle>
@@ -3333,6 +4287,508 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3840,13 +5296,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>82550</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3878,13 +5334,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>298450</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>6350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3916,13 +5372,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3954,13 +5410,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>298450</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3988,18 +5444,78 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="17" name="Chart 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C21B5954-1F15-FCD7-5B4E-EA9FD7FB183A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77AAA3D3-BC3B-3545-82AD-7DC4884D03E0}" name="Table1" displayName="Table1" ref="B2:F9" totalsRowShown="0">
-  <autoFilter ref="B2:F9" xr:uid="{77AAA3D3-BC3B-3545-82AD-7DC4884D03E0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{77AAA3D3-BC3B-3545-82AD-7DC4884D03E0}" name="Table1" displayName="Table1" ref="B3:F10" totalsRowShown="0">
+  <autoFilter ref="B3:F10" xr:uid="{77AAA3D3-BC3B-3545-82AD-7DC4884D03E0}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A4D967B2-2B6C-AD45-AB88-D5B191EAED50}" name="N"/>
     <tableColumn id="2" xr3:uid="{C9686C99-595A-4B44-92BB-115DD030649E}" name="Quadratic(ms)"/>
     <tableColumn id="3" xr3:uid="{D07CC844-2D5F-0147-BFE1-64AC089CA925}" name="Quadratic with Calipers(ms)"/>
     <tableColumn id="4" xr3:uid="{0020E07D-5460-CD48-AA22-E6F6A6909EBF}" name="Quadrithimic(ms)"/>
     <tableColumn id="5" xr3:uid="{C8B16365-8893-D244-9147-A718B07B8D6A}" name="Cubic(ms)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{66B9A91A-BDD7-5E4E-BDD5-8EBF23AAE195}" name="Table13" displayName="Table13" ref="H3:L10" totalsRowShown="0">
+  <autoFilter ref="H3:L10" xr:uid="{66B9A91A-BDD7-5E4E-BDD5-8EBF23AAE195}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{87D1A213-534F-0249-873A-A9B118E94470}" name="N">
+      <calculatedColumnFormula>LOG(Table1[[#This Row],[N]],2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{F0A0FB28-6E07-7146-B161-04F569847825}" name="Quadratic(ms)">
+      <calculatedColumnFormula>LOG(Table1[[#This Row],[Quadratic(ms)]],2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{5C31734C-B93A-9D46-A62B-5C1DF62789C9}" name="Quadratic with Calipers(ms)">
+      <calculatedColumnFormula>LOG(Table1[[#This Row],[Quadratic with Calipers(ms)]],2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{F7A1C2BE-363E-084B-B99E-8A768E07F697}" name="Quadrithimic(ms)">
+      <calculatedColumnFormula>LOG(Table1[[#This Row],[Quadrithimic(ms)]],2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{0FFD6AA2-37A7-2341-AC62-91862B266CFE}" name="Cubic(ms)">
+      <calculatedColumnFormula>LOG(Table1[[#This Row],[Cubic(ms)]],2)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4302,10 +5818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0652324E-9C2B-1C43-B0BB-047EA06BDF6E}">
-  <dimension ref="B2:F9"/>
+  <dimension ref="B1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+      <selection activeCell="F1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4316,144 +5832,315 @@
     <col min="6" max="6" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>3</v>
       </c>
+      <c r="H3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B4">
         <v>250</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>1.84</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>1.0900000000000001</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>1.08</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>5.97</v>
       </c>
+      <c r="H4">
+        <f>LOG(Table1[[#This Row],[N]],2)</f>
+        <v>7.965784284662087</v>
+      </c>
+      <c r="I4">
+        <f>LOG(Table1[[#This Row],[Quadratic(ms)]],2)</f>
+        <v>0.87970576628228825</v>
+      </c>
+      <c r="J4">
+        <f>LOG(Table1[[#This Row],[Quadratic with Calipers(ms)]],2)</f>
+        <v>0.12432813500220179</v>
+      </c>
+      <c r="K4">
+        <f>LOG(Table1[[#This Row],[Quadrithimic(ms)]],2)</f>
+        <v>0.11103131238874395</v>
+      </c>
+      <c r="L4">
+        <f>LOG(Table1[[#This Row],[Cubic(ms)]],2)</f>
+        <v>2.5777309314900805</v>
+      </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B5">
         <v>500</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>3.14</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>2.88</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>40.68</v>
       </c>
+      <c r="H5">
+        <f>LOG(Table1[[#This Row],[N]],2)</f>
+        <v>8.965784284662087</v>
+      </c>
+      <c r="I5">
+        <f>LOG(Table1[[#This Row],[Quadratic(ms)]],2)</f>
+        <v>1.6507645591169022</v>
+      </c>
+      <c r="J5">
+        <f>LOG(Table1[[#This Row],[Quadratic with Calipers(ms)]],2)</f>
+        <v>0.18903382439001684</v>
+      </c>
+      <c r="K5">
+        <f>LOG(Table1[[#This Row],[Quadrithimic(ms)]],2)</f>
+        <v>1.5260688116675876</v>
+      </c>
+      <c r="L5">
+        <f>LOG(Table1[[#This Row],[Cubic(ms)]],2)</f>
+        <v>5.3462477740827756</v>
+      </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B6">
         <v>1000</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>6.8</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>4.25</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>14.25</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>317.89999999999998</v>
       </c>
+      <c r="H6">
+        <f>LOG(Table1[[#This Row],[N]],2)</f>
+        <v>9.965784284662087</v>
+      </c>
+      <c r="I6">
+        <f>LOG(Table1[[#This Row],[Quadratic(ms)]],2)</f>
+        <v>2.7655347463629774</v>
+      </c>
+      <c r="J6">
+        <f>LOG(Table1[[#This Row],[Quadratic with Calipers(ms)]],2)</f>
+        <v>2.0874628412503395</v>
+      </c>
+      <c r="K6">
+        <f>LOG(Table1[[#This Row],[Quadrithimic(ms)]],2)</f>
+        <v>3.8328900141647417</v>
+      </c>
+      <c r="L6">
+        <f>LOG(Table1[[#This Row],[Cubic(ms)]],2)</f>
+        <v>8.3124292062506147</v>
+      </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B7">
         <v>2000</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>28.2</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>19</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>71.400000000000006</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>2518.6999999999998</v>
       </c>
+      <c r="H7">
+        <f>LOG(Table1[[#This Row],[N]],2)</f>
+        <v>10.965784284662087</v>
+      </c>
+      <c r="I7">
+        <f>LOG(Table1[[#This Row],[Quadratic(ms)]],2)</f>
+        <v>4.8176232575114311</v>
+      </c>
+      <c r="J7">
+        <f>LOG(Table1[[#This Row],[Quadratic with Calipers(ms)]],2)</f>
+        <v>4.2479275134435852</v>
+      </c>
+      <c r="K7">
+        <f>LOG(Table1[[#This Row],[Quadrithimic(ms)]],2)</f>
+        <v>6.1578521691417381</v>
+      </c>
+      <c r="L7">
+        <f>LOG(Table1[[#This Row],[Cubic(ms)]],2)</f>
+        <v>11.298463578910917</v>
+      </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B8">
         <v>4000</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>149.19999999999999</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>91.8</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>332.6</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>20007.599999999999</v>
       </c>
+      <c r="H8">
+        <f>LOG(Table1[[#This Row],[N]],2)</f>
+        <v>11.965784284662087</v>
+      </c>
+      <c r="I8">
+        <f>LOG(Table1[[#This Row],[Quadratic(ms)]],2)</f>
+        <v>7.2211037253678763</v>
+      </c>
+      <c r="J8">
+        <f>LOG(Table1[[#This Row],[Quadratic with Calipers(ms)]],2)</f>
+        <v>6.5204222485264456</v>
+      </c>
+      <c r="K8">
+        <f>LOG(Table1[[#This Row],[Quadrithimic(ms)]],2)</f>
+        <v>8.3776443583999072</v>
+      </c>
+      <c r="L8">
+        <f>LOG(Table1[[#This Row],[Cubic(ms)]],2)</f>
+        <v>14.288260499528787</v>
+      </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B9">
         <v>8000</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>686.67</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>527.66999999999996</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>1466.33</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>161619</v>
       </c>
+      <c r="H9">
+        <f>LOG(Table1[[#This Row],[N]],2)</f>
+        <v>12.965784284662087</v>
+      </c>
+      <c r="I9">
+        <f>LOG(Table1[[#This Row],[Quadratic(ms)]],2)</f>
+        <v>9.4234731247064101</v>
+      </c>
+      <c r="J9">
+        <f>LOG(Table1[[#This Row],[Quadratic with Calipers(ms)]],2)</f>
+        <v>9.0434921530640615</v>
+      </c>
+      <c r="K9">
+        <f>LOG(Table1[[#This Row],[Quadrithimic(ms)]],2)</f>
+        <v>10.517994105587512</v>
+      </c>
+      <c r="L9">
+        <f>LOG(Table1[[#This Row],[Cubic(ms)]],2)</f>
+        <v>17.30223728635373</v>
+      </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B10">
         <v>16000</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>2676.5</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>2263.5</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>6888</v>
+      </c>
+      <c r="F10">
+        <v>1285873</v>
+      </c>
+      <c r="H10">
+        <f>LOG(Table1[[#This Row],[N]],2)</f>
+        <v>13.965784284662087</v>
+      </c>
+      <c r="I10">
+        <f>LOG(Table1[[#This Row],[Quadratic(ms)]],2)</f>
+        <v>11.386131937314994</v>
+      </c>
+      <c r="J10">
+        <f>LOG(Table1[[#This Row],[Quadratic with Calipers(ms)]],2)</f>
+        <v>11.144339591247839</v>
+      </c>
+      <c r="K10">
+        <f>LOG(Table1[[#This Row],[Quadrithimic(ms)]],2)</f>
+        <v>12.749869427396845</v>
+      </c>
+      <c r="L10">
+        <f>LOG(Table1[[#This Row],[Cubic(ms)]],2)</f>
+        <v>20.294316730405338</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:L1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>